<commit_message>
Scale fix and other small fixes
</commit_message>
<xml_diff>
--- a/MUSIKKVIDEOUKA2025.xlsx
+++ b/MUSIKKVIDEOUKA2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/torgeir_bull_vestfoldfylke_no/Documents/Dokumenter/2025-2026/Annet/Musikkvideouka 2025/Musikkvideouka_V11_FIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DBB5177-76FE-47DE-AEE0-4ACA87ECD984}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E2D1FDB-54C1-4496-B646-FBD26CF92C77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Navn</t>
   </si>
@@ -31,111 +31,12 @@
     <t>Poeng</t>
   </si>
   <si>
-    <t>Gruppe 1</t>
-  </si>
-  <si>
-    <t>Gruppe 2</t>
-  </si>
-  <si>
-    <t>Gruppe 3</t>
-  </si>
-  <si>
-    <t>Gruppe 4</t>
-  </si>
-  <si>
-    <t>Gruppe 5</t>
-  </si>
-  <si>
-    <t>Gruppe 6</t>
-  </si>
-  <si>
-    <t>Gruppe 7</t>
-  </si>
-  <si>
-    <t>Gruppe 8</t>
-  </si>
-  <si>
-    <t>Gruppe 9</t>
-  </si>
-  <si>
-    <t>Gruppe 10</t>
-  </si>
-  <si>
-    <t>Gruppe 11</t>
-  </si>
-  <si>
-    <t>Gruppe 12</t>
-  </si>
-  <si>
-    <t>Gruppe 13</t>
-  </si>
-  <si>
-    <t>Gruppe 14</t>
-  </si>
-  <si>
-    <t>Gruppe 15</t>
-  </si>
-  <si>
-    <t>Gruppe 16</t>
-  </si>
-  <si>
-    <t>Gruppe 17</t>
-  </si>
-  <si>
-    <t>Gruppe 18</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_1.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_2.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_3.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_4.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_6.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_8.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_9.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_10.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_11.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_12.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_15.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_16.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_18.png</t>
-  </si>
-  <si>
-    <t>Gruppe 19</t>
-  </si>
-  <si>
     <t>/album_covers/artist_5.jpg</t>
   </si>
   <si>
     <t>/album_covers/artist_7.jpg</t>
   </si>
   <si>
-    <t>/album_covers/artist_13.jpg</t>
-  </si>
-  <si>
     <t>/album_covers/artist_14.jpg</t>
   </si>
   <si>
@@ -143,6 +44,93 @@
   </si>
   <si>
     <t>/album_covers/artist_19.jpg</t>
+  </si>
+  <si>
+    <t>Gruppe 2 - UMBRELLA</t>
+  </si>
+  <si>
+    <t>Gruppe 3 - I LOVE IT</t>
+  </si>
+  <si>
+    <t>Gruppe 4 - SLIM SHADY</t>
+  </si>
+  <si>
+    <t>Gruppe 5 - THAT’S WHAT IT IS</t>
+  </si>
+  <si>
+    <t>Gruppe 6 - PHOENIX</t>
+  </si>
+  <si>
+    <t>Gruppe 7 - AMERICAN IDIOT</t>
+  </si>
+  <si>
+    <t>Gruppe 8 - LOVE YOU LIKE A LOVE SONG</t>
+  </si>
+  <si>
+    <t>Gruppe 9 - THE DINER</t>
+  </si>
+  <si>
+    <t>Gruppe 10 - MOVES LIKE JAGGER</t>
+  </si>
+  <si>
+    <t>Gruppe 11 - NOW OR NEVER</t>
+  </si>
+  <si>
+    <t>Gruppe 12 - ON THE FLOOR</t>
+  </si>
+  <si>
+    <t>Gruppe 14 - UPTOWN FUNK</t>
+  </si>
+  <si>
+    <t>Gruppe 15 - ROCKY</t>
+  </si>
+  <si>
+    <t>Gruppe 16 - I’M STILL STANDING</t>
+  </si>
+  <si>
+    <t>Gruppe 17 - HOTEL ROOM SERVICE</t>
+  </si>
+  <si>
+    <t>Gruppe 18 - HER</t>
+  </si>
+  <si>
+    <t>Gruppe 19 - DRACULA</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_2.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_3.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_4.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_6.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_8.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_9.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_10.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_11.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_12.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_15.png</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_16.jpg</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_18.jpg</t>
   </si>
 </sst>
 </file>
@@ -561,15 +549,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.69921875" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -587,10 +575,10 @@
     </row>
     <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -598,10 +586,10 @@
     </row>
     <row r="3" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -609,10 +597,10 @@
     </row>
     <row r="4" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -620,10 +608,10 @@
     </row>
     <row r="5" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -631,10 +619,10 @@
     </row>
     <row r="6" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -642,10 +630,10 @@
     </row>
     <row r="7" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -653,10 +641,10 @@
     </row>
     <row r="8" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -664,10 +652,10 @@
     </row>
     <row r="9" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -675,10 +663,10 @@
     </row>
     <row r="10" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -686,10 +674,10 @@
     </row>
     <row r="11" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -697,10 +685,10 @@
     </row>
     <row r="12" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -708,10 +696,10 @@
     </row>
     <row r="13" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -719,10 +707,10 @@
     </row>
     <row r="14" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -730,10 +718,10 @@
     </row>
     <row r="15" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -741,10 +729,10 @@
     </row>
     <row r="16" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -752,10 +740,10 @@
     </row>
     <row r="17" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -763,45 +751,23 @@
     </row>
     <row r="18" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A3 A2 A18 A11 A10 A6 A5 A4 A7 A8 A9 A12 A13 A14 A15 A16 A17" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add vinner-overlay styles for winner announcement feature
- Introduced styles for the vinner-overlay background and main container.
- Styled various components including image box, name box, points box, and top 3 placement boxes.
- Added responsive design elements and visual enhancements such as shadows and borders.
</commit_message>
<xml_diff>
--- a/MUSIKKVIDEOUKA2025.xlsx
+++ b/MUSIKKVIDEOUKA2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/torgeir_bull_vestfoldfylke_no/Documents/Dokumenter/2025-2026/Annet/Musikkvideouka 2025/Musikkvideouka_V11_FIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E2D1FDB-54C1-4496-B646-FBD26CF92C77}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E31AF578-54D4-4D7A-AEC3-7EDAB3600D9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,10 +127,10 @@
     <t>/album_covers/gruppe_15.png</t>
   </si>
   <si>
-    <t>/album_covers/gruppe_16.jpg</t>
-  </si>
-  <si>
-    <t>/album_covers/gruppe_18.jpg</t>
+    <t>/album_covers/artist_16.jpg</t>
+  </si>
+  <si>
+    <t>/album_covers/gruppe_18.png</t>
   </si>
 </sst>
 </file>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>